<commit_message>
Importação dos acervos onomástico e temático
Importação dos acervos onomástico e temático
</commit_message>
<xml_diff>
--- a/mapeamento separado/CA mapeamento importação Acervo_Acessorio_de_armaria.xlsx
+++ b/mapeamento separado/CA mapeamento importação Acervo_Acessorio_de_armaria.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denni\Desktop\mdjvi-master\mapeamento separado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denni\Desktop\projeto\mdjvi-master\mapeamento separado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CE4598-2A6C-459B-9B92-CF3F73593A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5005900-C911-440C-811F-F7AB66D0E23F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>